<commit_message>
Added code to generate individual stock price graphs for 2008 and 2020, saved outputs to output folder.
</commit_message>
<xml_diff>
--- a/data_files/internet_sources/30Companies.xlsx
+++ b/data_files/internet_sources/30Companies.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06e891e7ad7d67e2/Rutgers Bootcamp/Projects/Project 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/06e891e7ad7d67e2/Rutgers Bootcamp/Projects/Project 1/Repository/data_files/internet_sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{BADA922F-EC55-4F05-8437-7D0E2F441614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{89312C79-B748-4F15-BF3C-160CBC735EE3}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="8_{BADA922F-EC55-4F05-8437-7D0E2F441614}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0EE83EEA-1647-4022-899F-F1EC6719A0E6}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{1C83C502-439E-47D8-8D81-44A73CA85D52}"/>
+    <workbookView xWindow="3030" yWindow="1725" windowWidth="30720" windowHeight="5700" xr2:uid="{1C83C502-439E-47D8-8D81-44A73CA85D52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>Symbol</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>E*Trade</t>
-  </si>
-  <si>
-    <t>AET</t>
   </si>
   <si>
     <t>Aetna Inc</t>
@@ -615,7 +612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEE00E5-C80F-4B25-ACE5-3A44FF312390}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -637,32 +636,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -670,65 +669,65 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
         <v>16</v>
@@ -747,225 +746,228 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="C14" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>27</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
         <v>43</v>
       </c>
-      <c r="B20" t="s">
-        <v>44</v>
-      </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" t="s">
         <v>47</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>49</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C27" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="C28" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B29" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C30" t="s">
-        <v>69</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B31" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C31">
+    <sortCondition ref="A2:A31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>